<commit_message>
BOM is fixed, Im sorry for that scam link.
Hopefully nobody bought that arduino pro mini.
</commit_message>
<xml_diff>
--- a/circadian rev2.0/circad 2.0 bom.xlsx
+++ b/circadian rev2.0/circad 2.0 bom.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eurorack-master\circadyan rhythms clone\code rev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6899131F-87DA-4FF2-AF4F-AA01F51B390F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6945862D-5EE0-4422-BDF3-384532F0EE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Braids v5.1" sheetId="4" r:id="rId1"/>
+    <sheet name="circad rev2.0" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="107">
   <si>
     <t>Index</t>
   </si>
@@ -156,9 +158,6 @@
     <t>capacitor</t>
   </si>
   <si>
-    <t>C1 - C12, C25, C26</t>
-  </si>
-  <si>
     <t>C24</t>
   </si>
   <si>
@@ -339,13 +338,22 @@
     <t>S73</t>
   </si>
   <si>
-    <t>rotary encoder w/ button</t>
-  </si>
-  <si>
     <t>U$4</t>
   </si>
   <si>
     <t>173.97mm x 111.43mm ; 2 layers</t>
+  </si>
+  <si>
+    <t>C1 - C12, C23,C25, C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">806-KUSBX-SMTBS1NB30 </t>
+  </si>
+  <si>
+    <t>rotary encoder w/ button (D shaft)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">688-EC11E18244A5 </t>
   </si>
 </sst>
 </file>
@@ -561,6 +569,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -570,8 +580,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8" hidden="1"/>
@@ -986,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z38"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1006,15 +1014,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1052,14 +1060,14 @@
       <c r="S2" s="22"/>
     </row>
     <row r="3" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="3"/>
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
@@ -1088,7 +1096,7 @@
       <c r="F4" s="13">
         <v>3535</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="26" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="22"/>
@@ -1121,7 +1129,7 @@
       <c r="F5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="26" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="22"/>
@@ -1153,7 +1161,7 @@
       <c r="F6" s="15">
         <v>603</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
@@ -1168,14 +1176,14 @@
       <c r="S6" s="22"/>
     </row>
     <row r="7" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="24"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
@@ -1266,7 +1274,7 @@
       <c r="F10" s="13">
         <v>603</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
@@ -1282,7 +1290,7 @@
     </row>
     <row r="11" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
@@ -1291,12 +1299,12 @@
         <v>40</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="13">
         <v>603</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -1312,7 +1320,7 @@
     </row>
     <row r="12" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="B12" s="13">
         <v>14</v>
@@ -1326,7 +1334,7 @@
       <c r="F12" s="13">
         <v>603</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
@@ -1342,7 +1350,7 @@
     </row>
     <row r="13" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="13">
         <v>2</v>
@@ -1351,12 +1359,12 @@
         <v>40</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="13">
         <v>603</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
@@ -1372,19 +1380,19 @@
     </row>
     <row r="14" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="G14" s="27"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
@@ -1400,21 +1408,21 @@
     </row>
     <row r="15" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="13">
         <v>2</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="13">
         <v>1206</v>
       </c>
-      <c r="G15" s="30"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
@@ -1430,22 +1438,22 @@
     </row>
     <row r="16" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="13">
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="13">
         <v>603</v>
       </c>
-      <c r="G16" s="30"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -1461,22 +1469,22 @@
     </row>
     <row r="17" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="13">
         <v>1</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="13">
         <v>603</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="22"/>
@@ -1492,16 +1500,18 @@
     </row>
     <row r="18" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="20"/>
-      <c r="G18" s="30"/>
+      <c r="G18" s="26" t="s">
+        <v>104</v>
+      </c>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="22"/>
@@ -1517,22 +1527,22 @@
     </row>
     <row r="19" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="13">
         <v>4</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>61</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>62</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -1549,7 +1559,7 @@
     </row>
     <row r="20" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -1558,15 +1568,15 @@
         <v>23</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
@@ -1582,7 +1592,7 @@
     </row>
     <row r="21" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
@@ -1591,15 +1601,15 @@
         <v>23</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="30"/>
+        <v>67</v>
+      </c>
+      <c r="G21" s="27"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
       <c r="J21" s="22"/>
@@ -1615,22 +1625,22 @@
     </row>
     <row r="22" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="13">
         <v>2</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="G22" s="27"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="J22" s="22"/>
@@ -1646,22 +1656,22 @@
     </row>
     <row r="23" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="13">
         <v>2</v>
       </c>
       <c r="C23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="G23" s="27"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="22"/>
@@ -1677,22 +1687,22 @@
     </row>
     <row r="24" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="13">
         <v>1</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="G24" s="27"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
       <c r="J24" s="22"/>
@@ -1708,22 +1718,22 @@
     </row>
     <row r="25" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="13">
         <v>1</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" s="30"/>
+        <v>71</v>
+      </c>
+      <c r="G25" s="27"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
@@ -1739,22 +1749,22 @@
     </row>
     <row r="26" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="13">
         <v>1</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>82</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>83</v>
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="30"/>
+        <v>83</v>
+      </c>
+      <c r="G26" s="27"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
@@ -1770,22 +1780,22 @@
     </row>
     <row r="27" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="30"/>
+        <v>91</v>
+      </c>
+      <c r="G27" s="27"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
@@ -1801,22 +1811,22 @@
     </row>
     <row r="28" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="13">
         <v>1</v>
       </c>
       <c r="C28" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>90</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>91</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="G28" s="27"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
@@ -1832,20 +1842,20 @@
     </row>
     <row r="29" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="13">
         <v>2</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E29" s="20"/>
+      <c r="G29" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="G29" s="29" t="s">
-        <v>96</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -1861,14 +1871,14 @@
       <c r="S29" s="22"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="25"/>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -1885,7 +1895,7 @@
     </row>
     <row r="31" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="13">
         <v>8</v>
@@ -1900,10 +1910,10 @@
         <v>13</v>
       </c>
       <c r="F31" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="26" t="s">
         <v>99</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>100</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -1920,7 +1930,7 @@
     </row>
     <row r="32" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="15">
         <v>20</v>
@@ -1944,15 +1954,18 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33" s="15">
         <v>1</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -1992,7 +2005,7 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="17">
         <v>1</v>
@@ -2033,7 +2046,7 @@
       <c r="E36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="G36" s="23" t="s">
+      <c r="G36" s="26" t="s">
         <v>20</v>
       </c>
       <c r="H36" s="22"/>
@@ -2066,12 +2079,18 @@
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12"/>
       <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B39" s="15">
+        <f>SUM(B4:B6,B8:B29,B31:B33,B35:B36)</f>
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2088,9 +2107,11 @@
     <hyperlink ref="G36" r:id="rId5" xr:uid="{26FEAA19-46DD-43FE-96BC-CBA17BF2DF7F}"/>
     <hyperlink ref="G19" r:id="rId6" xr:uid="{ADBD33F0-2969-49EF-81CC-8E8BBA8769D5}"/>
     <hyperlink ref="G29" r:id="rId7" xr:uid="{B22A27C8-2430-4F29-9CC7-84D89F2D12D8}"/>
+    <hyperlink ref="G18" r:id="rId8" xr:uid="{2C37FF28-C183-4A6E-923F-A6F3B580DC93}"/>
+    <hyperlink ref="G33" r:id="rId9" xr:uid="{AE1D874C-39F6-451D-B0E9-A9123F033D3A}"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId8"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>